<commit_message>
REbuilt thinner total size, swivel bars
</commit_message>
<xml_diff>
--- a/sPhenixTileTestStand.xlsx
+++ b/sPhenixTileTestStand.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\oneDrive\projects\sPhenixTileTestStand\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sawaiz\OneDrive\projects\sPhenixTileTestStand\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>parameter</t>
   </si>
@@ -35,40 +35,25 @@
     <t>unit</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>mm</t>
   </si>
   <si>
-    <t>ul</t>
-  </si>
-  <si>
     <t>note</t>
   </si>
   <si>
-    <t>plateWidth</t>
-  </si>
-  <si>
-    <t>plateDepth</t>
-  </si>
-  <si>
-    <t>supportPlateWidth</t>
-  </si>
-  <si>
-    <t>supportPlateThickness</t>
-  </si>
-  <si>
-    <t>supportPlateFillet</t>
-  </si>
-  <si>
-    <t>separation</t>
-  </si>
-  <si>
-    <t>numPanels</t>
-  </si>
-  <si>
-    <t>centerVerticalRatio</t>
+    <t>height</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>suppourtPlateLength</t>
+  </si>
+  <si>
+    <t>acrylicThickness</t>
   </si>
 </sst>
 </file>
@@ -78,7 +63,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,7 +98,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,7 +416,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,37 +437,37 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3">
         <v>300</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>0.25</v>
+        <v>150</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -490,58 +475,34 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2">
-        <v>50</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>10</v>
+        <v>3.125</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="2">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
+      <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>

</xml_diff>